<commit_message>
power and cooling parameters (research study)
</commit_message>
<xml_diff>
--- a/curve_fitting/curve_fitting_mod_config.xlsx
+++ b/curve_fitting/curve_fitting_mod_config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vemanuele/Desktop/regressione/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vemanuele/Documents/GitHub/masters-degree-thesis/curve_fitting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4BD3AF-B746-324C-A575-3A5C4165AD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83FAEFB-1C21-454E-940D-61C9DA6F86E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="1820" windowWidth="22160" windowHeight="16140" xr2:uid="{F1D764B0-189E-5E40-8AF6-304EF3F09BE8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="15420" windowHeight="16320" xr2:uid="{F1D764B0-189E-5E40-8AF6-304EF3F09BE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -174,6 +174,12 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.6602362204724412E-2"/>
+                  <c:y val="-0.59406787693205021"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -206,10 +212,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$A$19</c:f>
+              <c:f>Sheet1!$A$1:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>3000</c:v>
                 </c:pt>
@@ -256,82 +262,64 @@
                   <c:v>48000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>51000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>54000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>57000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>60000</c:v>
+                  <c:v>50000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$19</c:f>
+              <c:f>Sheet1!$B$1:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.09</c:v>
+                  <c:v>5.87</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.47</c:v>
+                  <c:v>4.2300000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.66</c:v>
+                  <c:v>3.45</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.18</c:v>
+                  <c:v>2.99</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.85</c:v>
+                  <c:v>2.69</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.62</c:v>
+                  <c:v>2.48</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.4500000000000002</c:v>
+                  <c:v>2.3199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.31</c:v>
+                  <c:v>2.2000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.21</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.08</c:v>
+                  <c:v>1.98</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.99</c:v>
+                  <c:v>1.9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.93</c:v>
+                  <c:v>1.86</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.89</c:v>
+                  <c:v>1.82</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.85</c:v>
+                  <c:v>1.78</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.82</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.79</c:v>
-                </c:pt>
-                <c:pt idx="17">
                   <c:v>1.76</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.73</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -339,7 +327,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A2B8-0A4A-BAA1-CE64FE8CF39A}"/>
+              <c16:uniqueId val="{00000000-9186-784C-8114-AFE03637A3F2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -351,11 +339,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="77084975"/>
-        <c:axId val="404868207"/>
+        <c:axId val="2141037872"/>
+        <c:axId val="2140957456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77084975"/>
+        <c:axId val="2141037872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -412,12 +400,12 @@
             <a:endParaRPr lang="en-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404868207"/>
+        <c:crossAx val="2140957456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="404868207"/>
+        <c:axId val="2140957456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -474,7 +462,7 @@
             <a:endParaRPr lang="en-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77084975"/>
+        <c:crossAx val="2141037872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1091,22 +1079,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>4993</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>3006</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>449493</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>104606</xdr:rowOff>
+      <xdr:colOff>463550</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B08B0CBB-1449-0814-F24E-DA8EF5E39904}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DF0C96B-2C69-B717-640A-E94B58A945C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1424,10 +1412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19F58D36-05D4-E847-BFF8-1D97C0A089FB}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1437,7 +1425,7 @@
         <v>3000</v>
       </c>
       <c r="B1">
-        <v>11</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1445,7 +1433,7 @@
         <v>6000</v>
       </c>
       <c r="B2">
-        <v>6.09</v>
+        <v>5.87</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1453,7 +1441,7 @@
         <v>9000</v>
       </c>
       <c r="B3">
-        <v>4.47</v>
+        <v>4.2300000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1461,7 +1449,7 @@
         <v>12000</v>
       </c>
       <c r="B4">
-        <v>3.66</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1469,7 +1457,7 @@
         <v>15000</v>
       </c>
       <c r="B5">
-        <v>3.18</v>
+        <v>2.99</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1477,7 +1465,7 @@
         <v>18000</v>
       </c>
       <c r="B6">
-        <v>2.85</v>
+        <v>2.69</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1485,7 +1473,7 @@
         <v>21000</v>
       </c>
       <c r="B7">
-        <v>2.62</v>
+        <v>2.48</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1493,7 +1481,7 @@
         <v>24000</v>
       </c>
       <c r="B8">
-        <v>2.4500000000000002</v>
+        <v>2.3199999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1501,7 +1489,7 @@
         <v>27000</v>
       </c>
       <c r="B9">
-        <v>2.31</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1509,7 +1497,7 @@
         <v>30000</v>
       </c>
       <c r="B10">
-        <v>2.21</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1517,7 +1505,7 @@
         <v>35000</v>
       </c>
       <c r="B11">
-        <v>2.08</v>
+        <v>1.98</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1525,7 +1513,7 @@
         <v>39000</v>
       </c>
       <c r="B12">
-        <v>1.99</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1533,7 +1521,7 @@
         <v>42000</v>
       </c>
       <c r="B13">
-        <v>1.93</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1541,7 +1529,7 @@
         <v>45000</v>
       </c>
       <c r="B14">
-        <v>1.89</v>
+        <v>1.82</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1549,39 +1537,15 @@
         <v>48000</v>
       </c>
       <c r="B15">
-        <v>1.85</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>51000</v>
+        <v>50000</v>
       </c>
       <c r="B16">
-        <v>1.82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>54000</v>
-      </c>
-      <c r="B17">
-        <v>1.79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>57000</v>
-      </c>
-      <c r="B18">
         <v>1.76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>60000</v>
-      </c>
-      <c r="B19">
-        <v>1.73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
attack scenario modeling, PUE formula approximation (research study)
</commit_message>
<xml_diff>
--- a/curve_fitting/curve_fitting_mod_config.xlsx
+++ b/curve_fitting/curve_fitting_mod_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vemanuele/Documents/GitHub/masters-degree-thesis/curve_fitting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83FAEFB-1C21-454E-940D-61C9DA6F86E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5824F1DF-329E-3846-B442-B648F45A7407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="15420" windowHeight="16320" xr2:uid="{F1D764B0-189E-5E40-8AF6-304EF3F09BE8}"/>
   </bookViews>
@@ -100,6 +100,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Curve fitting (modified</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -176,8 +206,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="4.6602362204724412E-2"/>
-                  <c:y val="-0.59406787693205021"/>
+                  <c:x val="0.12715791776027996"/>
+                  <c:y val="-0.73295676582093905"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1415,7 +1445,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>